<commit_message>
Updated Sprint 2 backlog
This commit involves revisions or modifications to the Sprint 2 backlog, likely including additions, removals, or updates to user stories, tasks, priorities, or estimates.
The changes made reflect the ongoing development progress or adjustments in project requirements, ensuring alignment with the current sprint goals and priorities.
</commit_message>
<xml_diff>
--- a/sprints/sprint2/sprint2_backlog.xlsx
+++ b/sprints/sprint2/sprint2_backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jgain\OneDrive\Documents\School\Spring 2024\UWG-SE2-Group5-Myst\sprints\sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7F656F-B6C0-464C-BC94-4C59AB0775E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79DD961-75AF-4F62-B67B-2412E4F9F1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,7 +398,7 @@
                   <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>25</c:v>
@@ -1448,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1527,7 +1527,9 @@
       <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
@@ -1542,7 +1544,9 @@
       <c r="D5" s="2">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
@@ -1557,7 +1561,9 @@
       <c r="D6" s="2">
         <v>3</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
@@ -1572,7 +1578,9 @@
       <c r="D7" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
@@ -1587,7 +1595,9 @@
       <c r="D8" s="2">
         <v>3</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
@@ -1602,7 +1612,9 @@
       <c r="D9" s="2">
         <v>3</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
@@ -1617,7 +1629,9 @@
       <c r="D10" s="2">
         <v>3</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>3</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
@@ -1632,7 +1646,9 @@
       <c r="D11" s="2">
         <v>3</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
@@ -1647,7 +1663,9 @@
       <c r="D12" s="2">
         <v>3</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
@@ -1662,7 +1680,9 @@
       <c r="D13" s="2">
         <v>3</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
@@ -1677,7 +1697,9 @@
       <c r="D14" s="2">
         <v>3</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
@@ -1692,7 +1714,9 @@
       <c r="D15" s="2">
         <v>3</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2">
+        <v>2</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
@@ -1707,7 +1731,9 @@
       <c r="D16" s="2">
         <v>3</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2">
+        <v>3</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
@@ -1875,7 +1901,9 @@
       <c r="D26" s="2">
         <v>3</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
@@ -1890,7 +1918,9 @@
       <c r="D27" s="2">
         <v>3</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
@@ -1905,7 +1935,9 @@
       <c r="D28" s="2">
         <v>3</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2">
+        <v>2</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
@@ -1920,7 +1952,9 @@
       <c r="D29" s="2">
         <v>3</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2">
+        <v>2</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
@@ -1935,7 +1969,9 @@
       <c r="D30" s="2">
         <v>3</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2">
+        <v>3</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
@@ -1950,7 +1986,9 @@
       <c r="D31" s="2">
         <v>3</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2">
+        <v>3</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
@@ -1965,7 +2003,9 @@
       <c r="D32" s="2">
         <v>3</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
@@ -1980,7 +2020,9 @@
       <c r="D33" s="2">
         <v>3</v>
       </c>
-      <c r="E33" s="2"/>
+      <c r="E33" s="2">
+        <v>2</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
@@ -1995,7 +2037,9 @@
       <c r="D34" s="2">
         <v>3</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="2">
+        <v>2</v>
+      </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
@@ -2010,7 +2054,9 @@
       <c r="D35" s="2">
         <v>3</v>
       </c>
-      <c r="E35" s="2"/>
+      <c r="E35" s="2">
+        <v>3</v>
+      </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
@@ -2025,7 +2071,9 @@
       <c r="D36" s="2">
         <v>3</v>
       </c>
-      <c r="E36" s="2"/>
+      <c r="E36" s="2">
+        <v>3</v>
+      </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
@@ -2105,7 +2153,7 @@
       </c>
       <c r="E44" s="3">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="F44" s="3">
         <f t="shared" si="0"/>

</xml_diff>